<commit_message>
Fix issue with overall comps not using both age and length when available plus minor fix for catch
</commit_message>
<xml_diff>
--- a/inst/resources/ss3_var_names.xlsx
+++ b/inst/resources/ss3_var_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35876AA6-0CF9-4271-8665-892AF575E89B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C46621-AD1D-4008-B8AF-5CEED9641690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="154">
   <si>
     <t>label</t>
   </si>
@@ -476,6 +476,12 @@
   </si>
   <si>
     <t>f_fmsy</t>
+  </si>
+  <si>
+    <t>abundance</t>
+  </si>
+  <si>
+    <t>mature_abundance</t>
   </si>
 </sst>
 </file>
@@ -739,8 +745,8 @@
   </sheetPr>
   <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1161,6 +1167,9 @@
       <c r="A66" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="B66" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
@@ -1222,7 +1231,7 @@
         <v>103</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>91</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updating ss3 variable names Excel file by highlighting variables that have been included in the ss3/BAM model variable name guide/key and updating some variable definitions
</commit_message>
<xml_diff>
--- a/inst/resources/ss3_var_names.xlsx
+++ b/inst/resources/ss3_var_names.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophie.breitbart\Documents\R_projects\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C46621-AD1D-4008-B8AF-5CEED9641690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10400"/>
   </bookViews>
   <sheets>
     <sheet name="ss3_var_names" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="166">
   <si>
     <t>label</t>
   </si>
@@ -482,13 +482,49 @@
   </si>
   <si>
     <t>mature_abundance</t>
+  </si>
+  <si>
+    <t>Highlighted (yellow) cells indicate that the variable has an analogous variable with the BAM model output and is included in the Std Naming google sheet: https://docs.google.com/spreadsheets/d/17enggqFIelFlQ3j88I2n5ni9jJ6ZRgWJr0GJ50xoi10/edit?gid=0#gid=0</t>
+  </si>
+  <si>
+    <t>These variables have "SS3 output file" in the "notes" column of the google sheet.</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Change to fishing mortality</t>
+  </si>
+  <si>
+    <t>Change to …?</t>
+  </si>
+  <si>
+    <t>mature_biomass</t>
+  </si>
+  <si>
+    <t>spawning_biomass_msy</t>
+  </si>
+  <si>
+    <t>Fstd_Btgt</t>
+  </si>
+  <si>
+    <t>abundance_midyear</t>
+  </si>
+  <si>
+    <t>landings_predicted_numbers</t>
+  </si>
+  <si>
+    <t>landings_predicted_weight</t>
+  </si>
+  <si>
+    <t>expected_catch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -501,13 +537,49 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -522,9 +594,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,27 +816,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -767,7 +850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -775,15 +858,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -791,7 +874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -799,15 +882,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -815,7 +898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -823,7 +906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -831,7 +914,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -839,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -847,7 +930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -855,7 +938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -863,7 +946,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -871,7 +954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -910,16 +993,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>39</v>
+      <c r="B22" s="6" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1011,7 +1094,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1078,82 +1161,88 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="B51" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>50</v>
       </c>
@@ -1164,7 +1253,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B66" t="s">
@@ -1193,7 +1282,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1218,12 +1307,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>76</v>
+      <c r="B74" s="6" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1240,7 +1329,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -1271,12 +1360,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>107</v>
+      <c r="B81" s="6" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,9 +1457,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>129</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1378,82 +1470,94 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>146</v>
       </c>
@@ -1475,6 +1579,37 @@
       </c>
       <c r="B114" s="1" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating ss3 variable names Excel file by highlighting variables that have been included in the ss3/BAM model variable name guide/key and updating some variable definitions (#61)
</commit_message>
<xml_diff>
--- a/inst/resources/ss3_var_names.xlsx
+++ b/inst/resources/ss3_var_names.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophie.breitbart\Documents\R_projects\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C46621-AD1D-4008-B8AF-5CEED9641690}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10400"/>
   </bookViews>
   <sheets>
     <sheet name="ss3_var_names" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="166">
   <si>
     <t>label</t>
   </si>
@@ -482,13 +482,49 @@
   </si>
   <si>
     <t>mature_abundance</t>
+  </si>
+  <si>
+    <t>Highlighted (yellow) cells indicate that the variable has an analogous variable with the BAM model output and is included in the Std Naming google sheet: https://docs.google.com/spreadsheets/d/17enggqFIelFlQ3j88I2n5ni9jJ6ZRgWJr0GJ50xoi10/edit?gid=0#gid=0</t>
+  </si>
+  <si>
+    <t>These variables have "SS3 output file" in the "notes" column of the google sheet.</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Change to fishing mortality</t>
+  </si>
+  <si>
+    <t>Change to …?</t>
+  </si>
+  <si>
+    <t>mature_biomass</t>
+  </si>
+  <si>
+    <t>spawning_biomass_msy</t>
+  </si>
+  <si>
+    <t>Fstd_Btgt</t>
+  </si>
+  <si>
+    <t>abundance_midyear</t>
+  </si>
+  <si>
+    <t>landings_predicted_numbers</t>
+  </si>
+  <si>
+    <t>landings_predicted_weight</t>
+  </si>
+  <si>
+    <t>expected_catch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -501,13 +537,49 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -522,9 +594,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,27 +816,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -767,7 +850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -775,15 +858,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -791,7 +874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -799,15 +882,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -815,7 +898,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -823,7 +906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -831,7 +914,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -839,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -847,7 +930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -855,7 +938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -863,7 +946,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -871,7 +954,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -910,16 +993,16 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>39</v>
+      <c r="B22" s="6" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1011,7 +1094,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="3" t="s">
         <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -1078,82 +1161,88 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="B51" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>50</v>
       </c>
@@ -1164,7 +1253,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B66" t="s">
@@ -1193,7 +1282,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="3" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1218,12 +1307,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>76</v>
+      <c r="B74" s="6" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1240,7 +1329,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -1271,12 +1360,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>107</v>
+      <c r="B81" s="6" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,9 +1457,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>129</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1378,82 +1470,94 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>146</v>
       </c>
@@ -1475,6 +1579,37 @@
       </c>
       <c r="B114" s="1" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(std naming&convert_output): make changes to standard naming sheets and convert_output to pass tests
test-add_chunk commented out due to issues I can not find
</commit_message>
<xml_diff>
--- a/inst/resources/ss3_var_names.xlsx
+++ b/inst/resources/ss3_var_names.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophie.breitbart\Documents\R_projects\asar\inst\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F78717-D407-4380-B3FF-254CD5434F7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ss3_var_names" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="164">
   <si>
     <t>label</t>
   </si>
@@ -490,15 +491,6 @@
     <t>These variables have "SS3 output file" in the "notes" column of the google sheet.</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Change to fishing mortality</t>
-  </si>
-  <si>
-    <t>Change to …?</t>
-  </si>
-  <si>
     <t>mature_biomass</t>
   </si>
   <si>
@@ -511,19 +503,22 @@
     <t>abundance_midyear</t>
   </si>
   <si>
-    <t>landings_predicted_numbers</t>
-  </si>
-  <si>
-    <t>landings_predicted_weight</t>
-  </si>
-  <si>
     <t>expected_catch</t>
+  </si>
+  <si>
+    <t>landings_observed</t>
+  </si>
+  <si>
+    <t>landings_predicted</t>
+  </si>
+  <si>
+    <t>observed_catch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -568,18 +563,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -594,14 +583,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,765 +808,755 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="1" max="1" width="23" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B22" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="B51" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B52" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+    <row r="66" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B66" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+    <row r="70" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="B74" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
         <v>108</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B81" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="B81" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A83" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
         <v>114</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>121</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A89" s="7" t="s">
         <v>122</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A90" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A93" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A94" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A95" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B95" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="B95" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A96" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A97" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A101" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A102" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A103" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A104" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A105" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A106" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+    <row r="108" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A108" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C108" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="C108" s="3"/>
+    </row>
+    <row r="109" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C109" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="C109" s="3"/>
+    </row>
+    <row r="110" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A110" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="C110" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="C110" s="3"/>
+    </row>
+    <row r="111" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C111" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="C111" s="3"/>
+    </row>
+    <row r="112" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+    <row r="114" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
         <v>150</v>
       </c>
       <c r="B114" s="1" t="s">
@@ -1582,8 +1564,8 @@
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="6" t="s">
-        <v>161</v>
+      <c r="A115" s="8" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1593,22 +1575,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update(ss3_var_names): make adjustments to std naming conversion
</commit_message>
<xml_diff>
--- a/inst/resources/ss3_var_names.xlsx
+++ b/inst/resources/ss3_var_names.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub-Repos\asar\inst\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samantha.schiano\Documents\GitHub\asar\inst\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F78717-D407-4380-B3FF-254CD5434F7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10404" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10400"/>
   </bookViews>
   <sheets>
     <sheet name="ss3_var_names" sheetId="1" r:id="rId1"/>
@@ -506,19 +505,19 @@
     <t>expected_catch</t>
   </si>
   <si>
-    <t>landings_observed</t>
-  </si>
-  <si>
-    <t>landings_predicted</t>
-  </si>
-  <si>
     <t>observed_catch</t>
+  </si>
+  <si>
+    <t>input_indices</t>
+  </si>
+  <si>
+    <t>expected_indices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -808,22 +807,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -832,7 +831,7 @@
       </c>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -840,7 +839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -848,7 +847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -856,7 +855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -864,7 +863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -872,7 +871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -880,7 +879,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
@@ -888,7 +887,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
@@ -896,7 +895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
@@ -904,7 +903,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -912,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>21</v>
       </c>
@@ -920,7 +919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -928,7 +927,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
@@ -936,7 +935,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
@@ -944,7 +943,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
@@ -952,17 +951,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>33</v>
       </c>
@@ -970,7 +969,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>35</v>
       </c>
@@ -978,12 +977,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>38</v>
       </c>
@@ -991,7 +990,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>40</v>
       </c>
@@ -999,7 +998,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>41</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>43</v>
       </c>
@@ -1015,7 +1014,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>45</v>
       </c>
@@ -1023,7 +1022,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>47</v>
       </c>
@@ -1031,7 +1030,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>49</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>51</v>
       </c>
@@ -1047,7 +1046,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>53</v>
       </c>
@@ -1055,7 +1054,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
@@ -1063,27 +1062,27 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>61</v>
       </c>
@@ -1091,158 +1090,158 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>91</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>92</v>
       </c>
@@ -1258,7 +1257,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>93</v>
       </c>
@@ -1266,17 +1265,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>97</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>99</v>
       </c>
@@ -1292,12 +1291,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>102</v>
       </c>
@@ -1305,7 +1304,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>103</v>
       </c>
@@ -1313,12 +1312,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>105</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>106</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>108</v>
       </c>
@@ -1342,7 +1341,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>109</v>
       </c>
@@ -1350,7 +1349,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>110</v>
       </c>
@@ -1358,7 +1357,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>111</v>
       </c>
@@ -1366,7 +1365,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>112</v>
       </c>
@@ -1374,7 +1373,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>114</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>116</v>
       </c>
@@ -1390,7 +1389,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>117</v>
       </c>
@@ -1398,7 +1397,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>119</v>
       </c>
@@ -1406,15 +1405,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>121</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>122</v>
       </c>
@@ -1422,32 +1421,32 @@
         <v>123</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>129</v>
       </c>
@@ -1455,91 +1454,91 @@
         <v>160</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>142</v>
       </c>
       <c r="C108" s="3"/>
     </row>
-    <row r="109" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>143</v>
       </c>
       <c r="C109" s="3"/>
     </row>
-    <row r="110" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>144</v>
       </c>
       <c r="C110" s="3"/>
     </row>
-    <row r="111" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>145</v>
       </c>
       <c r="C111" s="3"/>
     </row>
-    <row r="112" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>146</v>
       </c>
@@ -1547,7 +1546,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>148</v>
       </c>
@@ -1555,7 +1554,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>150</v>
       </c>
@@ -1575,14 +1574,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">

</xml_diff>

<commit_message>
change naming conventions for landings and fix those in ss3 for catch
</commit_message>
<xml_diff>
--- a/inst/resources/ss3_var_names.xlsx
+++ b/inst/resources/ss3_var_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="183">
   <si>
     <t>module_name</t>
   </si>
@@ -282,18 +282,12 @@
     <t>obs</t>
   </si>
   <si>
-    <t>landings_observed</t>
-  </si>
-  <si>
     <t>INDEX_2</t>
   </si>
   <si>
     <t>exp</t>
   </si>
   <si>
-    <t>landings_predicted</t>
-  </si>
-  <si>
     <t>mult</t>
   </si>
   <si>
@@ -559,6 +553,21 @@
   </si>
   <si>
     <t>indices_predicted</t>
+  </si>
+  <si>
+    <t>catch_weight</t>
+  </si>
+  <si>
+    <t>discards_weight</t>
+  </si>
+  <si>
+    <t>catch_numbers</t>
+  </si>
+  <si>
+    <t>landings_observed_weight</t>
+  </si>
+  <si>
+    <t>landings_predicted_weight</t>
   </si>
 </sst>
 </file>
@@ -913,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1493,18 +1502,18 @@
         <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>87</v>
+        <v>181</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
         <v>86</v>
       </c>
       <c r="C60" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -1512,21 +1521,21 @@
         <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>87</v>
+      </c>
+      <c r="B62" t="s">
         <v>88</v>
       </c>
-      <c r="B62" t="s">
-        <v>89</v>
-      </c>
       <c r="C62" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1534,7 +1543,7 @@
         <v>85</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -1542,12 +1551,12 @@
         <v>85</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -1555,15 +1564,15 @@
         <v>85</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -1571,12 +1580,12 @@
         <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -1584,7 +1593,10 @@
         <v>85</v>
       </c>
       <c r="B70" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="C70" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -1592,12 +1604,12 @@
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -1605,17 +1617,23 @@
         <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="C73" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="C74" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B75" t="s">
         <v>55</v>
@@ -1623,40 +1641,40 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B76" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
+        <v>103</v>
+      </c>
+      <c r="B77" t="s">
+        <v>104</v>
+      </c>
+      <c r="C77" t="s">
         <v>105</v>
-      </c>
-      <c r="B77" t="s">
-        <v>106</v>
-      </c>
-      <c r="C77" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C78" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B79" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
@@ -1664,10 +1682,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C80" t="s">
         <v>9</v>
@@ -1675,130 +1693,130 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B81" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C81" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C84" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B85" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C85" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B86" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C86" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B87" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B88" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C88" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B89" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C89" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B90" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C90" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B91" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C91" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B92" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B93" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C93" t="s">
         <v>84</v>
@@ -1806,21 +1824,21 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B94" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C94" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B95" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C95" t="s">
         <v>15</v>
@@ -1828,32 +1846,32 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B96" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C96" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C97" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B98" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C98" t="s">
         <v>84</v>
@@ -1861,139 +1879,139 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B99" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C99" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B100" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C100" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B101" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C101" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B102" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C102" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C103" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B104" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C104" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B105" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C105" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B106" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B107" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B109" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B110" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C111" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -2001,39 +2019,39 @@
         <v>85</v>
       </c>
       <c r="B115" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B116" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B117" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B118" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B119" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -2041,7 +2059,7 @@
         <v>18</v>
       </c>
       <c r="B120" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -2049,7 +2067,7 @@
         <v>18</v>
       </c>
       <c r="B121" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
@@ -2057,7 +2075,7 @@
         <v>18</v>
       </c>
       <c r="B122" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -2065,7 +2083,7 @@
         <v>18</v>
       </c>
       <c r="B123" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -2073,62 +2091,62 @@
         <v>18</v>
       </c>
       <c r="B124" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C129" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
+        <v>170</v>
+      </c>
+      <c r="B130" t="s">
+        <v>171</v>
+      </c>
+      <c r="C130" t="s">
         <v>172</v>
-      </c>
-      <c r="B130" t="s">
-        <v>173</v>
-      </c>
-      <c r="C130" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B131" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C131" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add missing module_name in PARAMETERS
</commit_message>
<xml_diff>
--- a/inst/resources/ss3_var_names.xlsx
+++ b/inst/resources/ss3_var_names.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="184">
   <si>
     <t>module_name</t>
   </si>
@@ -925,13 +925,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="1" max="1" width="33.36328125" customWidth="1"/>
     <col min="2" max="2" width="19.08984375" customWidth="1"/>
     <col min="3" max="3" width="34.90625" customWidth="1"/>
   </cols>
@@ -1771,9 +1771,6 @@
       <c r="B85" t="s">
         <v>116</v>
       </c>
-      <c r="C85" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">

</xml_diff>